<commit_message>
- Load testing.xlsx done - Fix bug when LoadTester.exe exit for zero number cpu
</commit_message>
<xml_diff>
--- a/iSpring/Load testing.xlsx
+++ b/iSpring/Load testing.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>При нормальных условиях</t>
   </si>
@@ -48,14 +48,47 @@
     <t>30 Мб, 31 слайд</t>
   </si>
   <si>
-    <t>При 1 свободном процессоре и 256 оперативной памяти</t>
+    <t>Состояние</t>
+  </si>
+  <si>
+    <t>корректно</t>
+  </si>
+  <si>
+    <t>Комментарий</t>
+  </si>
+  <si>
+    <t>В первые 10 секунд были подвисания, power point не отвечал</t>
+  </si>
+  <si>
+    <t>Так как нагрузка при увеличении размера презентации не меняется, не имеет смысла тестировать на презентациях более 300 слайдов</t>
+  </si>
+  <si>
+    <t>При 1 свободном процессоре и 256 Мб оперативной памяти</t>
+  </si>
+  <si>
+    <t>Около 3 секунд были подвисания, power point не отвечал</t>
+  </si>
+  <si>
+    <t>Около 6 секунд были подвисания, power point не отвечал</t>
+  </si>
+  <si>
+    <t>Около 12 секунд были подвисания, power point не отвечал</t>
+  </si>
+  <si>
+    <t>Около 5 секунд были подвисания, power point не отвечал</t>
+  </si>
+  <si>
+    <t>Один загруженный процессор это 25% от 100% ресурсов проыессоров</t>
+  </si>
+  <si>
+    <t>При меньших ресурсах не имеет смысла тестировать, так как не хватит ресуров даже на открытия окна Publish</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,13 +97,37 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -85,21 +142,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -394,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A5:H17"/>
+  <dimension ref="A5:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D14" sqref="D14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -408,32 +488,33 @@
     <col min="5" max="5" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:8">
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="1:12">
+      <c r="A5" s="4"/>
+      <c r="B5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="21" customHeight="1">
+    <row r="7" spans="1:12" ht="21" customHeight="1">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -443,17 +524,18 @@
       <c r="C7">
         <v>32</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>32</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>32</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -470,82 +552,177 @@
         <v>280</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="B9" s="2" t="s">
+    <row r="9" spans="1:12" ht="42.75" customHeight="1">
+      <c r="A9" s="4"/>
+      <c r="B9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="B12" s="2" t="s">
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:12" ht="49.5" customHeight="1">
+      <c r="A11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:12" ht="40.5" customHeight="1">
+      <c r="A12" s="4"/>
+      <c r="B12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="B15" s="2" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="1:12" ht="15" customHeight="1">
+      <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
+      <c r="B13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="1:12" ht="59.25" customHeight="1">
+      <c r="A14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:12" ht="42" customHeight="1">
+      <c r="A15" s="4"/>
+      <c r="B15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" ht="45.75" customHeight="1">
+      <c r="A17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1"/>
+    <row r="20" spans="1:5" ht="33.75" customHeight="1"/>
+    <row r="22" spans="1:5">
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B15:E15"/>
+  <mergeCells count="14">
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F13:L14"/>
     <mergeCell ref="B12:E12"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="F11:L11"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F12:L12"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>